<commit_message>
ler arquivos de imagens
</commit_message>
<xml_diff>
--- a/job_info.xlsx
+++ b/job_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,222 +478,222 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fram Capital</t>
+          <t>Artesanal Investimentos</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estagiário Financeiro</t>
+          <t>Estágio de Risco - Mercado Financeiro (Presencial)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vila Nova Conceição – Zona Sul</t>
+          <t>Não informado</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cursando Engenharias, a partir do 5º semestre, entendimento acerca de contabilidade (balanço, DRE, etc)</t>
+          <t>Microsoft Excel, Conhecimentos em Lógica de Programação, Cursando os últimos 4 semestres de engenharias, matemática, estatística, economia ou física</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Bolsa Auxílio R$2.600,00 + Vale Refeição R$600,00</t>
+          <t>Plataforma Educacional, Clínica Corporativa, Gympass, VT sem desconto ou estacionamento, Assistência Médica, Vale Refeição, Cartão Flash, Sala de Leitura, Auxílio Creche, Empréstimo Consignado, Freshbox, Bônus</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Interessados enviar CV com o assunto “Financeiro” para jcosta@framcapital.com</t>
+          <t>Estudantes a partir do 5º semestre de engenharias, matemática, estatística, economia ou física</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Financeira</t>
+          <t>Risco - Mercado Financeiro</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Rotinas Administrativas; Emissão de Notas Fiscais; Contas a pagar; Contas a receber; Atualização de sistema financeiro; Conciliação Bancária; Automatização de Processos.</t>
+          <t>Processamento do cálculo de risco das carteiras dos fundos, Análise de risco, Condução e atualização de apresentações para o Comitê Risco, Monitoramento da performance dos ativos da carteira e dos fundos.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Paggo (Stealth Startup)</t>
+          <t>Consultoria no setor de saúde.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Estagiário em Engenharia de Software</t>
+          <t>Estágio.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Remoto</t>
+          <t>Não especificada.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Adquirir conhecimento e proficiência no trabalho com as stacks de tecnologia mais modernas do mercado, desenvolver produtos de software usando melhores práticas de lógica e programação, influenciar o desenvolvimento de produto, entendendo alavancas de geração de valor para nossos clientes.</t>
+          <t>Formação em Engenharia, Administração ou Economia, Conhecimento do Pacote Office, Boa capacidade de comunicação, Perfil focado, dinâmico e com capacidade analítica.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 3.900,00, divididos da seguinte forma: R$ 3000,00 (contrato de estágio), R$ 900,00 em um cartão de benefícios flexíveis.</t>
+          <t>Bolsa competitiva com política de bônus agressiva.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Jovens brilhantes e ambiciosos, que queiram acelerar suas carreiras e aprender em um ritmo extremamente desafiador e recompensador.</t>
+          <t>Não especificado.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Engenharia de Software</t>
+          <t>Modelagem financeira, Estruturação e otimização de processos, Interação direta com os clientes.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Adquirir conhecimento e proficiência no trabalho com as stacks de tecnologia mais modernas do mercado, desenvolver produtos de software usando melhores práticas de lógica e programação, influenciar o desenvolvimento de produto, entendendo alavancas de geração de valor para nossos clientes.</t>
+          <t>Não especificadas.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Grupo Boticário</t>
+          <t>Finlead</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pessoa Desenvolvedora BackEnd Java/Kotlin Especialista II (Produtos Digitais Financeiros)</t>
+          <t>Estagiário para área de Análise de Investimentos e Controle de Operações</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Remoto</t>
+          <t>Não mencionado</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Experiência com soluções cloud AWS, conhecimento em Python, JavaScript/TypeScript(Node) e/ou Java/Kotlin, interesse e conhecimento em estruturas de dados, experiência com monitoração e logging, conhecimento de Rest e orientação a eventos(Kafka), experiência com testes unitários e de integração, ponto de vista crítico quanto à performance e segurança, domínio do git ou outro sistema de controle de versão colaborativo, conhecimento em CI / CD, conhecimento em serverless framework, familiaridade em banco de dados relacional e não relacional, conhecimento em produtos financeiros voltados à créditos, capacidade de conduzir root cause analysis em problemas de software, experiência com testes de carga.</t>
+          <t>Proatividade, perfil analítico e quantitativo, conhecimento avançado em Excel e matemática financeira, conclusão da graduação em Engenharia ou finanças até julho de 2026, bom conhecimento em finanças, inglês avançado, conhecimentos de controladoria de fundos e regulamentação aplicável à gestão de fundos de investimento, domínio do pacote Office.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>A combinar</t>
+          <t>Bolsa competitiva ao mercado, Vale Refeição, Vale Transporte</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pessoas com deficiência, pessoas negras (pretas e pardas), mulheres (cis e trans), pessoas da comunidade LGBTQIA+ e pessoas 50+.</t>
+          <t>Estudantes de graduação em Engenharia ou finanças, preferencialmente nos cursos de administração, ciências contábeis ou economia, com conclusão prevista até julho de 2026.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tecnologia, Finanças</t>
+          <t>Análise de Investimentos e Controle de Operações</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Atuar como especialista em desenvolvimento de soluções em nuvem, projetar e implementar arquiteturas escaláveis e seguras na AWS, participar do desenho da arquitetura de solução, desenvolver e manter uma base de código de alta qualidade, investigar e resolver problemas técnicos complexos, se manter atualizado sobre as últimas tendências e tecnologias, avaliar impactos, riscos e estimativa de esforços, colaborar com equipes multifuncionais para definir requisitos técnicos, fornecer orientação técnica e suporte à equipe.</t>
+          <t>Auxiliar na elaboração de relatórios, monitorar aderência das compras às regras do fundo, auxiliar no monitoramento do fluxo de caixa, preparar relatórios gerenciais, acompanhar originações e administração dos investidores e mediadores, integrar com a área de investimentos do fundo para operações, acompanhar novas ações e desempenho da carteira.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BTG Pactual</t>
+          <t>Jera Capital Family Office</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Estágio Short - Automation 2024</t>
+          <t>Estágio</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Remoto</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Estar cursando regularmente um curso de formação superior (nível bacharel ou tecnólogo), possuir um computador com conexão à internet, ter disponibilidade de trabalhar no mínimo 2 meses, disponibilidade para trabalhar presencialmente no escritório de São Paulo ou Rio de Janeiro em caso de efetivação, conhecimento em base lógica de programação.</t>
+          <t>Inglês avançado ou fluente, graduação em andamento nas áreas de Economia, Administração, Engenharia ou áreas correlatas, Python Intermediário, Pacote Office Avançado (VBA), disponibilidade para modelo de trabalho (3x presencial na semana).</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>A combinar</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Estudantes com formação superior em andamento</t>
+          <t>Estudantes de graduação nas áreas de Economia, Administração, Engenharia ou áreas correlatas</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Área de Automation</t>
+          <t>Gestão, automatização de processos e rotinas</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Desenvolver automações, construir telas de front-end em ReactJS e Flask, programar back-end e APIs de serviços em Python, criar processos padronizados, lidar com diversos tipos de produtos financeiros, desenvolver soluções definidas, prestar suporte, manter relacionamento com os usuários, negociar prioridade das soluções, documentar processos e soluções, acompanhar o time de Discovery no mapeamento de processos, desenvolver soluções de alto impacto, garantir a estabilidade e o funcionamento das soluções do time.</t>
+          <t>Auxílio ao time nas atividades da área, busca de automatização dos processos e rotinas do dia a dia.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bain &amp; Company</t>
+          <t>Fram Capital</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AC - Associate Consultant (efetivo e fulltime), ACI - Associate Consultant Intern (estágio regular - 6 a 12 meses), Summer Associate Consultant Intern (estágio de férias - 8 a 12 semanas)</t>
+          <t>Estagiário Financeiro</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Remoto</t>
+          <t>Vila Nova Conceição – Zona Sul</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Estudante universitário ou recém formado, habilidades analíticas, interpessoais, criativas, de resolução de problemas e de liderança.</t>
+          <t>Cursando Engenharias, a partir do 5º semestre; Entendimento acerca de contabilidade (balanço, DRE, etc)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>A combinar</t>
+          <t>Bolsa Auxílio R$2.600,00; Vale Refeição R$600,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Estudantes universitários ou recém formados</t>
+          <t>Interessados enviar CV com o assunto “Financeiro” para jcosta@framcapital.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Consultoria estratégica</t>
+          <t>Rotinas Administrativas; Emissão de Notas Fiscais; Contas a pagar; Contas a receber; Atualização de sistema financeiro; Conciliação Bancária; Automatização de Processos.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Trabalhar em equipe, responsabilizar-se pela identificação de fontes de informação, coleta e interpretação de dados, apresentação dos resultados, entrevistar consumidores, fornecedores e empregadores, responsabilidade de supervisionar colegas mais novos após acumular experiência.</t>
+          <t>Não especificado no texto da vaga.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>+A Educação</t>
+          <t>Paggo (Stealth Startup)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Estágio em Talent Acquisition (Atração e Seleção)</t>
+          <t>Estagiário em Engenharia de Software</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -703,49 +703,49 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ensino Superior em andamento, habilidades com Pacote Office, disponibilidade para trabalho híbrido (se residir em Porto Alegre/RS), proatividade, comunicação, flexibilidade, organização e bom relacionamento interpessoal</t>
+          <t>Adquirir conhecimento e proficiência no trabalho com as stacks de tecnologia mais modernas do mercado, desenvolver produtos de software usando melhores práticas de lógica e programação, influenciar o desenvolvimento de produto, entendendo alavancas de geração de valor para nossos clientes.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>A combinar</t>
+          <t>R$ 3900,00 (R$ 3000,00 contrato de estágio + R$ 900,00 em um cartão de benefícios flexíveis)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Estudantes com Ensino Superior em andamento</t>
+          <t>Jovens brilhantes e ambiciosos</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Recursos Humanos, Atração e Seleção</t>
+          <t>Engenharia de Software</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Mapeamento de talentos, busca ativa de candidatos, alinhamento de perfil técnico e comportamental das vagas, divulgação, triagem, entrevistas, admissão de novos colaboradores, suporte em People Analytics e gestão de plataformas de seleção.</t>
+          <t>Adquirir conhecimento e proficiência no trabalho com as stacks de tecnologia mais modernas do mercado, desenvolver produtos de software usando melhores práticas de lógica e programação, influenciar o desenvolvimento de produto.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rehagro</t>
+          <t>Grupo Boticário</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Estágio - Área Comercial</t>
+          <t>Pessoa Desenvolvedora BackEnd Java/Kotlin Especialista II (Engenharia de Crédito) (Produtos Digitais Financeiros)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Remoto, com disponibilidade eventual de estar presente no laboratório nas unidades de MG ou SP</t>
+          <t>Remoto</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Estudante dos cursos de Ciências Agrárias, com conhecimento na área de interesse e vocação para a área comercial. Graduação em andamento, preferencialmente do 4º ao 8º período.</t>
+          <t>Experiência com soluções cloud AWS, conhecimento em Python, JavaScript/TypeScript(Node) e/ou Java/Kotlin, interesse e conhecimento em estruturas de dados, experiência com monitoração e logging, conhecimento de Rest e orientação a eventos(Kafka), experiência com testes unitários e de integração, ponto de vista crítico quanto à performance e segurança, visão de qualidade de software, domínio do git ou outro sistema de controle de versão colaborativo, conhecimento em CI / CD, conhecimento em serverless framework, vivência em times ágeis (Scrum, Kanban, etc), familiaridade em banco de dados relacional e não relacional, conhecimento em produtos financeiros voltados à créditos, capacidade de conduzir root cause analysis em problemas de software, experiência com testes de carga.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -755,29 +755,29 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Estudantes dos cursos de Ciências Agrárias</t>
+          <t>Pessoas com deficiência, pessoas negras (pretas e pardas), mulheres (cis e trans), pessoas da comunidade LGBTQIA+ e pessoas 50+.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Área Comercial, Vendas Internas</t>
+          <t>Tecnologia, Produtos Digitais Financeiros</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Dar apoio nos processo de vendas internas, em atividades de contato direto com clientes, acompanhamento de pedidos e fornecimento de suporte ao pós-venda. Aprender sobre os produtos e serviços oferecidos pelo laboratório, bem como entender as necessidades e demandas dos clientes do setor de pecuária e agricultura.</t>
+          <t>Atuar como especialista em desenvolvimento de soluções em nuvem, liderar tecnicamente o desenvolvimento de soluções, projetar, implementar e manter arquiteturas escaláveis e seguras na AWS, participar do desenho da arquitetura de solução, participar das definições de novas features de produto, desenvolver e manter uma base de código de alta qualidade, resolver problemas técnicos complexos, se manter atualizado sobre as últimas tendências e tecnologias, avaliar impactos, riscos e estimativa de esforços, colaborar com equipes multifuncionais, fornecer orientação técnica e suporte à equipe.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Visagio</t>
+          <t>BTG Pactual</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Desenvolvedor(a) de Software</t>
+          <t>Estágio Short - Automation 2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Conhecimento básico em metodologias ágeis, padrões de projeto e arquitetura de sistemas; Conhecimento básico em pelo menos uma linguagem de programação (ex: C#, Kotlin, Ruby, etc.) e framework (ex: .NET, SpringBoot, Rails, etc.)</t>
+          <t>Cursando regularmente um curso de formação superior (nível bacharel ou tecnólogo), possui um computador com conexão à internet, disponibilidade de trabalhar no mínimo 2 meses, disponibilidade para trabalhar presencialmente em São Paulo ou Rio de Janeiro em caso de efetivação, conhecimento em base lógica de programação.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -797,29 +797,29 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Universitários dos cursos de Ciência da Computação, Engenharias, Sistemas de Informação e afins</t>
+          <t>Estudantes de curso superior (nível bacharel ou tecnólogo) com interesse em tecnologia e automação.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Engenharia de Dados, Automação de Processos, Gestão de TI e Desenvolvimento de Software</t>
+          <t>Automation</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Desenvolvimento front-end e/ou back-end; Correção de bugs e melhoria contínua; Definição de melhores tecnologias a serem usadas nos sistemas desenvolvidos; Propor e implementar novas ferramentas, técnicas e metodologias; Compartilhar e evoluir o conhecimento técnico do time.</t>
+          <t>Desenvolver automações, construir telas de front-end em ReactJS e Flask, programar back-end e APIs de serviços em Python, criar processos padronizados, lidar com produtos financeiros, desenvolver e garantir a qualidade das soluções, prestar suporte, manter um relacionamento próximo com os usuários, negociar prioridades, promover a missão da área, documentar processos e soluções, acompanhar o time de Discovery, desenvolver soluções de alto impacto e garantir a estabilidade das soluções do time.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Smarthis</t>
+          <t>Bain &amp; Company</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Programa de Estágio Smarthis 2024</t>
+          <t>AC - Associate Consultant (efetivo e fulltime), ACI - Associate Consultant Intern (estágio regular - 6 a 12 meses), Summer Associate Consultant Intern (estágio de férias - 8 a 12 semanas)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Graduação a partir do 6º período, Conhecimento em alguma linguagem de programação (.NET, Python, PHP, Java, C#, VBA, VB Script, entre outras), Inglês avançado, Conhecimento em Machine Learning, Business Intelligence ou RPA (Robotic Process Automation), Conhecimento em Excel.</t>
+          <t>Estudante universitário ou recém formado</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,29 +839,29 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Estudantes a partir do 6º período com conhecimentos específicos em programação e inglês avançado</t>
+          <t>Estudantes universitários ou recém formados</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>RPA (Robotic Process Automation), Data Analytics e Inteligência Artificial</t>
+          <t>Consultoria estratégica</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Contribuir para uma entrega de soluções de automação, ajudando aos nossos clientes nas suas transformações digitais.</t>
+          <t>Aplicar e desenvolver habilidades analíticas, interpessoais, criativas, de resolução de problemas e de liderança; trabalhar em equipe; responsabilizar-se pela identificação de fontes de informação, coleta e interpretação de dados, execução de análises e apresentação dos resultados; entrevistar consumidores dos clientes, concorrentes, fornecedores e empregadores; assumir a responsabilidade de supervisionar colegas mais novos do time.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Radix</t>
+          <t>+A Educação</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Estágio em Desenvolvimento de Negócios</t>
+          <t>Estágio em Talent Acquisition (Atração e Seleção)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Cursando Engenharia de Processos, Mecânica, Automação ou áreas correlatas com formação prevista para a partir de 2025/2; Inglês Avançado/Fluente; Excel Intermediário/Avançado; Capacidade de gerenciamento de tempo e resolução de problemas; Vontade de aprender e se desenvolver.</t>
+          <t>Ensino Superior em andamento, habilidades com Pacote Office, disponibilidade para trabalho híbrido se residir em Porto Alegre/RS, proatividade, comunicação, flexibilidade, organização e bom relacionamento interpessoal.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -881,59 +881,227 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Estudantes de Engenharia de Processos, Mecânica, Automação ou áreas correlatas</t>
+          <t>Estudantes com ensino superior em andamento</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Desenvolvimento de Negócios</t>
+          <t>Atração e Seleção</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Apoio no mapeamento e prospecção de oportunidades; Realização de pesquisas de mercado e ações de pré-venda; Elaboração e apresentação de propostas técnicas-comerciais; Acompanhamento da equipe técnica nas estimativas de recursos para projetos; Representação da empresa em visitas técnicas e reuniões; Apoio na construção, formalização e conclusão de propostas comerciais e orçamentárias; Elaboração de materiais de divulgação de soluções desenvolvidas pela empresa.</t>
+          <t>Mapeamento de talentos, atuar na busca ativa de candidatos, alinhar perfil técnico e comportamental das vagas, realização de entrevistas, auxílio no processo de admissão, apoio em People Analytics e gerenciamento de plataformas de seleção.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Rehagro</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Estágio - Área Comercial</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Remoto, com disponibilidade eventual para estar presente no laboratório nas unidades de MG ou SP</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Estudante dos cursos de Ciências Agrárias, preferencialmente do 4º ao 8º período, conhecimento na área de interesse, interesse em atuar na área comercial direcionada para Vendas Internas</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Estudantes dos cursos de Ciências Agrárias</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Área Comercial, Vendas Internas</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Apoio nos processos de vendas internas, atividades de contato direto com clientes, acompanhamento de pedidos, fornecimento de suporte ao pós-venda, aprender sobre os produtos e serviços oferecidos pelo laboratório.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Visagio</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Estágio: Desenvolvedor(a) de Software</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Conhecimento básico em metodologias ágeis, padrões de projeto e arquitetura de sistemas, conhecimento básico em pelo menos uma linguagem de programação (ex: C#, Kotlin, Ruby, etc.) e framework (ex: .NET, SpringBoot, Rails, etc.)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Universitários dos cursos de Ciência da Computação, Engenharias, Sistemas de Informação e afins</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Engenharia de Dados, Automação de Processos, Gestão de TI e Desenvolvimento de Software</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Desenvolvimento front-end e/ou back-end; Correção de bugs e melhoria contínua; Definição de melhores tecnologias a serem usadas nos sistemas desenvolvidos; Propor e implementar novas ferramentas, técnicas e metodologias; Compartilhar e evoluir o conhecimento técnico do time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Smarthis</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Programa de Estágio Smarthis 2024</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Graduação a partir do 6º período; conhecimento em alguma linguagem de programação (.NET, Python, PHP, Java, C#, VBA, VB Script, entre outras); inglês avançado</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Estudantes de graduação a partir do 6º período com interesse em tecnologia e conhecimento em programação</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>RPA (Robotic Process Automation), Business Analytics</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Desenvolver soluções em RPA em conjunto com seu time para clientes nacionais e/ou internacionais; contribuir para uma entrega de soluções de automação, ajudando aos nossos clientes nas suas transformações digitais.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Radix</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Estágio em Desenvolvimento de Negócios</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Estar cursando Engenharia de Processos, Mecânica, Automação ou áreas correlatas com formação prevista para a partir de 2025/2; Inglês Avançado/Fluente; Excel Intermediário/Avançado; Capacidade de gerenciamento de tempo e resolução de problemas; Vontade de aprender e se desenvolver. Diferencial: Conhecimentos da indústria de Óleo &amp; Gás, Conhecimentos básicos de automação.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Estudantes de Engenharia de Processos, Mecânica, Automação ou áreas correlatas</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Desenvolvimento de Negócios, Engenharia, Automação, Desenvolvimento de Software e Produtos, TI Industrial e Consultoria</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Apoiar no mapeamento e prospecção de oportunidades; Realizar pesquisas de mercado e ações de pré-venda; Elaborar e apresentar propostas técnicas-comerciais nas áreas de atuação da empresa; Acompanhar a equipe técnica nas estimativas de recursos para projetos; Representar a empresa em visitas técnicas e reuniões para a discussão de escopo de projetos; Apoiar na construção, formalização e conclusão de propostas comerciais e orçamentárias; Elaborar materiais de divulgação de soluções desenvolvidas pela Radix.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>Liv Up</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>Estágio em Growth - Business Intelligence</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Remoto (Anywhere Office, em qualquer lugar do Brasil)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Formatura a partir de Dez/25, capacidade de resolução de problemas de forma analítica e criativa, pró-atividade, boa comunicação, Excel &amp; PowerPoint avançado, Inglês avançado, SQL e Python são diferenciais</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Remoto (Anywhere Office), qualquer lugar do Brasil</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Formatura a partir de Dez/25, Capacidade de resolução de problemas de forma analítica e criativa, Pró atividade, ser mão-na-massa e ter alta capacidade de implementação, Boa comunicação, Excel &amp; PowerPoint avançado, Inglês avançado, SQL e Python são diferenciais</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>A combinar</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Estudantes com formatura a partir de Dez/25</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Growth, Business Intelligence</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Elaboração de modelos de projeção de receita e custos, elaboração de modelos de projeção por canais de marketing, resolução de problemas relacionados a múltiplas áreas, acompanhamento da performance de testes de Growth, identificação e automação de processos recorrentes, explicação de principais resultados, elaboração de planos de ação e apresentações.</t>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Business Intelligence, Growth, Estratégia de Crescimento, Marketing</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Elaborar modelos de projeção de receita e custos, Elaborar modelos de projeção por canais de marketing, Auxiliar na resolução de problemas relacionados a múltiplas áreas, Acompanhar a performance de testes de Growth, Capacidade de identificar processos recorrentes e automatizá-los, Explicar principais resultados, e alinhar planos de ação com os times responsáveis, Elaborar apresentações para explicar modelagem e resultados dos projetos a serem desenvolvidos.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mais exemplos de vagas
</commit_message>
<xml_diff>
--- a/job_info.xlsx
+++ b/job_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,12 +483,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Estágio de Risco - Mercado Financeiro (Presencial)</t>
+          <t>Estágio de Risco - Mercado Financeiro</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Não informado</t>
+          <t>Presencial</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -498,7 +498,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Plataforma Educacional, Clínica Corporativa, Gympass, VT sem desconto ou estacionamento, Assistência Médica, Vale Refeição, Cartão Flash, Sala de Leitura, Auxílio Creche, Empréstimo Consignado, Freshbox, Bônus</t>
+          <t>Plataforma Educacional, Clínica Corporativa, VT sem desconto ou estacionamento, Gympass, Assistência Médica, Vale Refeição, Cartão Flash, Sala de Leitura, Auxílio Creche, Empréstimo Consignado, Freshbook, Bônus</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -508,54 +508,54 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Risco - Mercado Financeiro</t>
+          <t>Mercado Financeiro, Risco</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Processamento do cálculo de risco das carteiras dos fundos, Análise de risco, Condução e atualização de apresentações para o Comitê Risco, Monitoramento da performance dos ativos da carteira e dos fundos.</t>
+          <t>Processamento do cálculo de risco das carteiras dos fundos, Análise de risco, Atualização de apresentações para o Comitê Risco, Monitoramento de garantias e resseguro.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Consultoria no setor de saúde.</t>
+          <t>Empresa de consultoria para o setor de saúde</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Estágio.</t>
+          <t>Estágio</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Não especificada.</t>
+          <t>Não mencionado</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Formação em Engenharia, Administração ou Economia, Conhecimento do Pacote Office, Boa capacidade de comunicação, Perfil focado, dinâmico e com capacidade analítica.</t>
+          <t>Formação em Engenharia, Administração ou Economia; Conhecimento do Pacote Office; Boa capacidade de comunicação; Perfil focado, dinâmico e com capacidade analítica</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Bolsa competitiva com política de bônus agressiva.</t>
+          <t>Bolsa competitiva com política de bônus agressiva</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Não especificado.</t>
+          <t>Não mencionado</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Modelagem financeira, Estruturação e otimização de processos, Interação direta com os clientes.</t>
+          <t>Consultoria, saúde, finanças</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Não especificadas.</t>
+          <t>Modelagem financeira, estruturação e otimização de processos, interação direta com os clientes.</t>
         </is>
       </c>
     </row>
@@ -567,17 +567,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Estagiário para área de Análise de Investimentos e Controle de Operações</t>
+          <t>Estágio em Análise de Investimentos e Controle de Operações</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Não mencionado</t>
+          <t>Não especificado</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Proatividade, perfil analítico e quantitativo, conhecimento avançado em Excel e matemática financeira, conclusão da graduação em Engenharia ou finanças até julho de 2026, bom conhecimento em finanças, inglês avançado, conhecimentos de controladoria de fundos e regulamentação aplicável à gestão de fundos de investimento, domínio do pacote Office.</t>
+          <t>Proatividade, perfil analítico e quantitativo, conhecimento avançado em Excel e matemática financeira, graduação em Engenharia ou finanças (preferencialmente administração, ciências contábeis ou economia), conhecimento em finanças, inglês avançado, conhecimento em controladoria de fundos e regulamentação aplicável à gestão de fundos de investimento, domínio do pacote Office</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -587,7 +587,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Estudantes de graduação em Engenharia ou finanças, preferencialmente nos cursos de administração, ciências contábeis ou economia, com conclusão prevista até julho de 2026.</t>
+          <t>Estudantes universitários em Engenharia ou Finanças</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -597,7 +597,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Auxiliar na elaboração de relatórios, monitorar aderência das compras às regras do fundo, auxiliar no monitoramento do fluxo de caixa, preparar relatórios gerenciais, acompanhar originações e administração dos investidores e mediadores, integrar com a área de investimentos do fundo para operações, acompanhar novas ações e desempenho da carteira.</t>
+          <t>Elaboração de relatórios, acompanhamento de aquisições, monitoramento de aderência de compras, preparação de relatórios gerenciais, atuação no relacionamento com empresas, integração com a originadora do fundo.</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Inglês avançado ou fluente, graduação em andamento nas áreas de Economia, Administração, Engenharia ou áreas correlatas, Python Intermediário, Pacote Office Avançado (VBA), disponibilidade para modelo de trabalho (3x presencial na semana).</t>
+          <t>Inglês Avançado ou Fluente, Graduação em andamento nas áreas de Economia, Administração, Engenharia ou áreas Correlatas, Python Intermediário, Pacote Office Avançado (VBA), Disponibilidade para modelo de trabalho (3x presencial na semana).</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -629,17 +629,17 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Estudantes de graduação nas áreas de Economia, Administração, Engenharia ou áreas correlatas</t>
+          <t>Estudantes nas áreas de Economia, Administração, Engenharia ou áreas Correlatas</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Gestão, automatização de processos e rotinas</t>
+          <t>Gestão de investimentos, Automatização de processos e rotinas diárias</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Auxílio ao time nas atividades da área, busca de automatização dos processos e rotinas do dia a dia.</t>
+          <t>Auxílio ao time, buscar automatizar os processos e rotinas do dia a dia, atuação 360° dentro da gestora.</t>
         </is>
       </c>
     </row>
@@ -661,12 +661,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cursando Engenharias, a partir do 5º semestre; Entendimento acerca de contabilidade (balanço, DRE, etc)</t>
+          <t>Cursando Engenharias, a partir do 5º semestre, entendimento acerca de contabilidade (balanço, DRE, etc)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bolsa Auxílio R$2.600,00; Vale Refeição R$600,00</t>
+          <t>Bolsa Auxílio R$2.600,00, Vale Refeição R$600,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -676,12 +676,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>Financeira</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>Rotinas Administrativas; Emissão de Notas Fiscais; Contas a pagar; Contas a receber; Atualização de sistema financeiro; Conciliação Bancária; Automatização de Processos.</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Não especificado no texto da vaga.</t>
         </is>
       </c>
     </row>
@@ -703,12 +703,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Adquirir conhecimento e proficiência no trabalho com as stacks de tecnologia mais modernas do mercado, desenvolver produtos de software usando melhores práticas de lógica e programação, influenciar o desenvolvimento de produto, entendendo alavancas de geração de valor para nossos clientes.</t>
+          <t>Adquirir conhecimento e proficiência no trabalho com as stacks de tecnologia mais modernas do mercado, desenvolver produtos de software usando melhores práticas de lógica e programação, influenciar o desenvolvimento de produto.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 3900,00 (R$ 3000,00 contrato de estágio + R$ 900,00 em um cartão de benefícios flexíveis)</t>
+          <t>R$ 3.900,00 (R$ 3000,00 contrato de estágio + R$ 900,00 em um cartão de benefícios flexíveis)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Experiência com soluções cloud AWS, conhecimento em Python, JavaScript/TypeScript(Node) e/ou Java/Kotlin, interesse e conhecimento em estruturas de dados, experiência com monitoração e logging, conhecimento de Rest e orientação a eventos(Kafka), experiência com testes unitários e de integração, ponto de vista crítico quanto à performance e segurança, visão de qualidade de software, domínio do git ou outro sistema de controle de versão colaborativo, conhecimento em CI / CD, conhecimento em serverless framework, vivência em times ágeis (Scrum, Kanban, etc), familiaridade em banco de dados relacional e não relacional, conhecimento em produtos financeiros voltados à créditos, capacidade de conduzir root cause analysis em problemas de software, experiência com testes de carga.</t>
+          <t>Experiência com soluções cloud AWS, conhecimento em Python, JavaScript/TypeScript(Node) e/ou Java/Kotlin, interesse e conhecimento em estruturas de dados, experiência com monitoração e logging, conhecimento de Rest e orientação a eventos(Kafka), experiência com testes unitários e de integração, visão de qualidade de software, domínio do git ou outro sistema de controle de versão colaborativo, conhecimento em CI / CD, conhecimento em serverless framework, familiaridade em banco de dados relacional e não relacional, conhecimento em produtos financeiros voltados à créditos, capacidade de conduzir root cause analysis em problemas de software, experiência com testes de carga.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -755,29 +755,29 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Pessoas com deficiência, pessoas negras (pretas e pardas), mulheres (cis e trans), pessoas da comunidade LGBTQIA+ e pessoas 50+.</t>
+          <t>Vagas destinadas aos grupos minorizados priorizados em nossa estratégia: pessoas com deficiência, pessoas negras (pretas e pardas), mulheres (cis e trans), pessoas da comunidade LGBTQIA+ e pessoas 50+.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Tecnologia, Produtos Digitais Financeiros</t>
+          <t>Desenvolvimento de Plataforma de Crédito, Produtos Digitais Financeiros.</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Atuar como especialista em desenvolvimento de soluções em nuvem, liderar tecnicamente o desenvolvimento de soluções, projetar, implementar e manter arquiteturas escaláveis e seguras na AWS, participar do desenho da arquitetura de solução, participar das definições de novas features de produto, desenvolver e manter uma base de código de alta qualidade, resolver problemas técnicos complexos, se manter atualizado sobre as últimas tendências e tecnologias, avaliar impactos, riscos e estimativa de esforços, colaborar com equipes multifuncionais, fornecer orientação técnica e suporte à equipe.</t>
+          <t>Participar do desenho da arquitetura de solução e cenários de uso, definir requisitos técnicos, arquitetura de sistemas e melhores abordagens de desenvolvimento, apoiar profissionais que precisem da sua experiência ou orientação, contribuir com os time de infraestrutura, segurança e arquitetura para determinar as melhores soluções para os problemas, fornecer orientação técnica e suporte à equipe, compartilhar conhecimento e melhores práticas, ajudar na evolução técnica dos outros desenvolvedores.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BTG Pactual</t>
+          <t>Cadastra</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Estágio Short - Automation 2024</t>
+          <t>Data Strategy Assistant - Estágio</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Cursando regularmente um curso de formação superior (nível bacharel ou tecnólogo), possui um computador com conexão à internet, disponibilidade de trabalhar no mínimo 2 meses, disponibilidade para trabalhar presencialmente em São Paulo ou Rio de Janeiro em caso de efetivação, conhecimento em base lógica de programação.</t>
+          <t>Habilidades de comunicação interpessoal, interesse em aprender e se desafiar, desejo de trabalhar em um ambiente dinâmico, matrícula ativa em um curso superior (tecnologia, administração, publicidade, marketing, engenharias ou áreas correlatas). Diferenciais: Conhecimentos básicos em Ferramentas de Analytics, Data Visualization, HTML e linguagens de programação (Javascript), conhecimento de métricas de marketing digital, GTM e tagueamento, inglês para leitura.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -797,29 +797,29 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Estudantes de curso superior (nível bacharel ou tecnólogo) com interesse em tecnologia e automação.</t>
+          <t>Estudantes com matrícula ativa em curso superior</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Automation</t>
+          <t>Data &amp; Analytics</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Desenvolver automações, construir telas de front-end em ReactJS e Flask, programar back-end e APIs de serviços em Python, criar processos padronizados, lidar com produtos financeiros, desenvolver e garantir a qualidade das soluções, prestar suporte, manter um relacionamento próximo com os usuários, negociar prioridades, promover a missão da área, documentar processos e soluções, acompanhar o time de Discovery, desenvolver soluções de alto impacto e garantir a estabilidade das soluções do time.</t>
+          <t>Participar de reuniões com clientes e equipes internas, responsável pela implementação, gestão e manutenção de tags e plataformas de Digital Analytics para Sites e Aplicativos, responsável pela criação e manutenção de bases de dados, responsável por criar documentos instrutivos de implementações para clientes, responsável por planejar e gerenciar o plano de métricas, auxiliar na confecção de dashboards e relatórios básicos para clientes, auxiliar no desenvolvimento de análises descritivas e diagnósticas para os clientes.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bain &amp; Company</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AC - Associate Consultant (efetivo e fulltime), ACI - Associate Consultant Intern (estágio regular - 6 a 12 meses), Summer Associate Consultant Intern (estágio de férias - 8 a 12 semanas)</t>
+          <t>Programa de Estágio Santander</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Estudante universitário ou recém formado</t>
+          <t>Ser estudante de graduação ou tecnólogo a partir do 2° semestre, disponibilidade para jornada de 4h ou 6h diárias, ser curioso, questionador e com vontade de transformar.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,29 +839,29 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Estudantes universitários ou recém formados</t>
+          <t>Estudantes de graduação ou tecnólogos a partir do 2° semestre</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Consultoria estratégica</t>
+          <t>Lojas, Corporativo, áreas de apoio (Tecnologia, Comunicação, Riscos, Jurídico, entre outras), Atacado.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Aplicar e desenvolver habilidades analíticas, interpessoais, criativas, de resolução de problemas e de liderança; trabalhar em equipe; responsabilizar-se pela identificação de fontes de informação, coleta e interpretação de dados, execução de análises e apresentação dos resultados; entrevistar consumidores dos clientes, concorrentes, fornecedores e empregadores; assumir a responsabilidade de supervisionar colegas mais novos do time.</t>
+          <t>Participação em projetos importantes para o banco, desenvolvimento de potencial em projetos que têm o poder de transformar o mercado, a sociedade e a vida de nossos clientes.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>+A Educação</t>
+          <t>Akross</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Estágio em Talent Acquisition (Atração e Seleção)</t>
+          <t>Estagiária em Desenvolvimento Backend</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ensino Superior em andamento, habilidades com Pacote Office, disponibilidade para trabalho híbrido se residir em Porto Alegre/RS, proatividade, comunicação, flexibilidade, organização e bom relacionamento interpessoal.</t>
+          <t>Cursando ensino superior em Ciência da Computação, Engenharia de Software, Sistemas de Informação, Análise e Desenvolvimento de Sistemas ou áreas correlatas; Formatura prevista a partir de Junho/2026; Conhecimento em Orientação a Objetos; Conhecimento em Java 8+ e Spring Boot; Conhecimento em Hibernate/JPA; Conhecimento em bancos de dados relacionais (MySQL, PostgreSQL) ou NoSQL (MongoDB); Capacidade de atuar em equipe e boa comunicação.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -881,39 +881,39 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Estudantes com ensino superior em andamento</t>
+          <t>Estudantes de Ciência da Computação, Engenharia de Software, Sistemas de Informação, Análise e Desenvolvimento de Sistemas ou áreas correlatas.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Atração e Seleção</t>
+          <t>Desenvolvimento Backend</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Mapeamento de talentos, atuar na busca ativa de candidatos, alinhar perfil técnico e comportamental das vagas, realização de entrevistas, auxílio no processo de admissão, apoio em People Analytics e gerenciamento de plataformas de seleção.</t>
+          <t>Participar de forma supervisionada no desenvolvimento de aplicações Java, sob arquitetura de microsserviços; Colaborar com a equipe de desenvolvimento em algumas fases do ciclo de vida do software; Contribuir com a documentação técnica dos sistemas e aplicações; Estar junto do time na resolução de problemas das aplicações para absorção de conhecimentos; Trabalhar com a metodologia ágil Scrum, participando ativamente das cerimônias.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Rehagro</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Estágio - Área Comercial</t>
+          <t>Estágio TI - Desenvolvimento</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Remoto, com disponibilidade eventual para estar presente no laboratório nas unidades de MG ou SP</t>
+          <t>Remoto (presencial na Honda Morumbi 1x por mês), São Paulo</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Estudante dos cursos de Ciências Agrárias, preferencialmente do 4º ao 8º período, conhecimento na área de interesse, interesse em atuar na área comercial direcionada para Vendas Internas</t>
+          <t>Cursando graduação em tecnologia da informação e correlatas; Conhecimento em Informática: Linguagens de programação: Java, Genexus, web banco de dados: DB2(AS400 e/ou AIX) e Cloud; Inglês intermediário.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -923,29 +923,29 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Estudantes dos cursos de Ciências Agrárias</t>
+          <t>Estudantes de graduação em tecnologia da informação e correlatas</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Área Comercial, Vendas Internas</t>
+          <t>TI, Desenvolvimento</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Apoio nos processos de vendas internas, atividades de contato direto com clientes, acompanhamento de pedidos, fornecimento de suporte ao pós-venda, aprender sobre os produtos e serviços oferecidos pelo laboratório.</t>
+          <t>Apoio na organização da entrega contínua dos produtos de software ou projetos de sistemas; Apoio aos times de desenvolvedores na aplicação das melhorias práticas e técnicas de codificação; Apoio na gestão dos fornecedores externos.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Visagio</t>
+          <t>Radix Engenharia e Software</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Estágio: Desenvolvedor(a) de Software</t>
+          <t>Estágio em Desenvolvimento de Software</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Conhecimento básico em metodologias ágeis, padrões de projeto e arquitetura de sistemas, conhecimento básico em pelo menos uma linguagem de programação (ex: C#, Kotlin, Ruby, etc.) e framework (ex: .NET, SpringBoot, Rails, etc.)</t>
+          <t>Cursando graduação em Ciência da Computação, Engenharia de Software, Sistemas de Informação ou áreas afins com previsão conclusão para 2026/1, conhecimento básico de programação em Python, familiaridade com JavaScript e frameworks frontend como React.js, desejo de aprender sobre bancos de dados NoSQL, especialmente MongoDB.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -965,29 +965,29 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Universitários dos cursos de Ciência da Computação, Engenharias, Sistemas de Informação e afins</t>
+          <t>Estudantes de graduação em Ciência da Computação, Engenharia de Software, Sistemas de Informação ou áreas afins</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Engenharia de Dados, Automação de Processos, Gestão de TI e Desenvolvimento de Software</t>
+          <t>Desenvolvimento de Software, Engenharia de Software, Sistemas de Informação</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Desenvolvimento front-end e/ou back-end; Correção de bugs e melhoria contínua; Definição de melhores tecnologias a serem usadas nos sistemas desenvolvidos; Propor e implementar novas ferramentas, técnicas e metodologias; Compartilhar e evoluir o conhecimento técnico do time.</t>
+          <t>Auxiliar no desenvolvimento e manutenção da infraestrutura backend utilizando Python e frameworks como Flask ou FastAPI, suportar a implementação e gerenciamento de bancos de dados MongoDB, participar do desenvolvimento de interfaces de usuário utilizando JavaScript, React.js, Node.js e Express, ajudar na utilização de Redux para gerenciamento de estado em aplicações React, colaborar com a equipe de desenvolvimento para resolver problemas e implementar melhorias, participar de reuniões e sessões de brainstorming para contribuir com ideias inovadoras, manter a documentação técnica organizada e atualizada.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Smarthis</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Programa de Estágio Smarthis 2024</t>
+          <t>Programa de Estágio Bradesco 2024 Atacado</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Graduação a partir do 6º período; conhecimento em alguma linguagem de programação (.NET, Python, PHP, Java, C#, VBA, VB Script, entre outras); inglês avançado</t>
+          <t>Estudante de nível superior (bacharelado, licenciatura ou tecnólogo), cursando a partir do 2º semestre da graduação ou do 1º semestre de tecnólogo; Disponibilidade para uma jornada de 20, 25 ou 30 horas semanais e, preferencialmente, com possibilidade de estagiar por 2 anos; Inglês a partir do nível intermediário</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1007,29 +1007,29 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Estudantes de graduação a partir do 6º período com interesse em tecnologia e conhecimento em programação</t>
+          <t>Estudantes de nível superior a partir do 2º semestre</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>RPA (Robotic Process Automation), Business Analytics</t>
+          <t>Área financeira, Atacado</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Desenvolver soluções em RPA em conjunto com seu time para clientes nacionais e/ou internacionais; contribuir para uma entrega de soluções de automação, ajudando aos nossos clientes nas suas transformações digitais.</t>
+          <t>Mergulhar no universo dos grandes investidores, desvendando as soluções financeiras mais inovadoras do mercado, atendimento a grandes investidores institucionais do Brasil e clientes de private banking.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Radix</t>
+          <t>Britvic Brasil</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Estágio em Desenvolvimento de Negócios</t>
+          <t>Estagiária em Comércio Exterior</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1039,69 +1039,489 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Estar cursando Engenharia de Processos, Mecânica, Automação ou áreas correlatas com formação prevista para a partir de 2025/2; Inglês Avançado/Fluente; Excel Intermediário/Avançado; Capacidade de gerenciamento de tempo e resolução de problemas; Vontade de aprender e se desenvolver. Diferencial: Conhecimentos da indústria de Óleo &amp; Gás, Conhecimentos básicos de automação.</t>
+          <t>Cursando Administração, Logística, Comércio Exterior, Relações Internacionais ou cursos afins; Conhecimento intermediário em Pacote Office - Word, Excel e Power Point; Conhecimento intermediário em inglês é desejável.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>A combinar</t>
+          <t>A combinar; Bolsa-Auxílio; Vale Transporte; Vale Refeição; Wellhub (gympass)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Estudantes de Engenharia de Processos, Mecânica, Automação ou áreas correlatas</t>
+          <t>Estudantes dos cursos mencionados nos requisitos</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Desenvolvimento de Negócios, Engenharia, Automação, Desenvolvimento de Software e Produtos, TI Industrial e Consultoria</t>
+          <t>Comércio Exterior, Administração, Logística, Relações Internacionais</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Apoiar no mapeamento e prospecção de oportunidades; Realizar pesquisas de mercado e ações de pré-venda; Elaborar e apresentar propostas técnicas-comerciais nas áreas de atuação da empresa; Acompanhar a equipe técnica nas estimativas de recursos para projetos; Representar a empresa em visitas técnicas e reuniões para a discussão de escopo de projetos; Apoiar na construção, formalização e conclusão de propostas comerciais e orçamentárias; Elaborar materiais de divulgação de soluções desenvolvidas pela Radix.</t>
+          <t>Acompanhamento do fluxo de exportação, preparação do pacote de documentos dos embarques, acompanhamento de coletas realizadas dentro do território brasileiro, responsável pelo fluxo de pagamentos dos fornecedores da logísticas.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>alt.bank</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Estagiária em Marketing</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Graduação em andamento em cursos correlatos a Publicação, Marketing ou Relações Públicas, habilidades de planejamento de comunicação e execução de redes sociais, aptidão para criar conteúdo envolvente para mídias sociais, experiência com algumas plataformas de mídia social relevantes (Facebook, Instagram e Tiktok), desejável experiência com Linkedin, Twitter e Pinterest, desejável ter seu próprio perfil relevante em alguma rede social, fortes habilidades de comunicação verbal e escrita em português, bom domínio da língua inglesa.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>A combinar, inclui bolsa estágio, vale alimentação/refeição, Gympass, plano de saúde e odontológico.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Estudantes de graduação em cursos correlatos a Publicação, Marketing ou Relações Públicas.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Marketing, Mídias Sociais.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Auxiliar na concepção e entrega de estratégias de mídia social, criar planejamento e calendário de postagens, publicar e dar manutenção nos conteúdos publicados nas redes sociais, auxiliar no desenvolvimento, lançamento e gerenciamento de novas campanhas, gerar relatórios e analisar o desempenho em plataformas de mídia social, auxiliar na identificação de tendências de consumo, ajudar a otimizar o conteúdo para incentivar a interação e o envolvimento da comunidade, pesquisar e avaliar as ferramentas e técnicas mais recentes para melhor medir a atividade nas redes sociais.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ACE Ventures</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Estagiário(a) de Consultoria - Estratégia e Inteligência</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Cursando graduação em Administração, Economia, Engenharia ou áreas relacionadas (a partir do 3º semestre); Interesse genuíno por empreendedorismo, inovação e novas tecnologias; Conhecimento em estratégia empresarial, pesquisa de mercado e análise de dados; Mente curiosa e analítica, com facilidade para identificar padrões e tendências; Excelente comunicação oral e escrita.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Estudantes a partir do 3º semestre dos cursos de Administração, Economia, Engenharia ou áreas relacionadas.</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Consultoria, Estratégia Corporativa, Pesquisa de Mercado, Análise de Empresas, Projetos de Consultoria.</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Auxiliar na formulação e implementação de estratégias corporativas; Conduzir pesquisas de mercado; Elaborar apresentações executivas; Organizar e gerenciar informações do projeto; Realizar análises financeiras e estratégicas de empresas; Participar de todas as etapas dos projetos de consultoria.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>BTG Pactual</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Estágio Short - Automation 2024</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Cursando regularmente um curso de formação superior (nível bacharel ou tecnólogo), possuir um computador com conexão à internet, disponibilidade para trabalhar no mínimo 2 meses, disponibilidade para trabalhar presencialmente em São Paulo ou Rio de Janeiro em caso de efetivação, conhecimento em base lógica de programação.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Estudantes de curso superior (nível bacharel ou tecnólogo)</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Automation</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Desenvolver automações, construir telas de front-end em ReactJS e Flask, programar back-end e APIs de serviços em Python, criar processos padronizados, lidar com produtos financeiros, desenvolver soluções definidas, prestar suporte, manter um relacionamento próximo com os usuários, negociar a prioridade das soluções, fomentar a missão da área, documentar os processos e soluções, acompanhar o time de Discovery, desenvolver soluções de alto impacto, garantir a estabilidade e o funcionamento das soluções do time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Arquivei</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Estágio em CRM (Marketing)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Estar cursando Ensino Superior nas áreas de marketing, engenharia, administração, data science, ou similares; habilidades de comunicação oral e escrita; habilidade para trabalhar com Google Sheet; Noções de marketing digital.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Estudantes de Ensino Superior nas áreas de marketing, engenharia, administração, data science, ou similares.</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Marketing, CRM.</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Auxiliar no planejamento, implementação e análise de desempenho de réguas de comunicação e campanhas; Auxiliar na criação de conteúdo das comunicações; Contribuir no desenvolvimento de relatórios de performance para identificação de oportunidades de otimização; Contribuir com o aumento da representatividade de CRM na geração de demanda para o time de vendas, e com a melhora das principais métricas de CRM.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Bain &amp; Company</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AC - Associate Consultant, ACI - Associate Consultant Intern, Summer Associate Consultant Intern</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Estudante universitário ou recém-formado, habilidades analíticas, interpessoais, criativas, de resolução de problemas e de liderança</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Estudantes universitários ou recém-formados</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Consultoria Estratégica</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Trabalho em equipe, identificação de fontes de informação, coleta e interpretação de dados, execução de análises, apresentação de resultados, entrevistas com consumidores, concorrentes, fornecedores e empregadores, supervisão de colegas mais novos.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>+A Educação</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Estágio em Talent Acquisition (Atração e Seleção)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Ensino Superior em andamento, habilidades com o Pacote Office, disponibilidade para atuar em formato de trabalho híbrido em Porto Alegre/RS ou remota em outros locais, proatividade, comunicação, flexibilidade, organização e bom relacionamento interpessoal.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Estudantes com ensino superior em andamento</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Recursos Humanos, área de Desenvolvimento, Atração e Seleção</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Mapeamento de talentos, busca ativa de candidatos, alinhamento de perfil das vagas, divulgação, triagem, entrevistas, processo de admissão de novos colaboradores, gestão das plataformas de seleção.</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Rehagro</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Estágio - Área Comercial</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Estudante dos cursos de Ciências Agrárias, conhecimento na área de interesse, vocação e vontade de se especializar na área comercial, disponibilidade de eventualmente estar presente no laboratório nas unidades de MG ou SP.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Estudantes dos cursos de Ciências Agrárias, preferencialmente do 4º ao 8º período</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Comercial, Vendas Internas, Ciências Agrárias</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Dar apoio nos processo de vendas internas, em atividades de contato direto com clientes, acompanhamento de pedidos e fornecimento de suporte ao pós-venda, aprender sobre os produtos e serviços oferecidos pelo laboratório, entender as necessidades e demandas dos clientes do setor de pecuária e agricultura.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Visagio</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Estágio Desenvolvedor(a) de Software</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Conhecimento básico em metodologias ágeis, padrões de projeto e arquitetura de sistemas; conhecimento básico em pelo menos uma linguagem de programação (ex: C#, Kotlin, Ruby, etc.) e framework (ex: .NET, SpringBoot, Rails, etc.)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Universitários dos cursos de Ciência da Computação, Engenharias, Sistemas de Informação e afins</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Engenharia de Dados, Automação de Processos, Gestão de TI e Desenvolvimento de Software</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Desenvolvimento front-end e/ou back-end; Correção de bugs e melhoria contínua; Definição de melhores tecnologias a serem usadas nos sistemas desenvolvidos; Propor e implementar novas ferramentas, técnicas e metodologias; Compartilhar e evoluir o conhecimento técnico do time.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Smarthis</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Programa de Estágio Smarthis 2024</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Graduação a partir do 6º período, conhecimento em alguma linguagem de programação (.NET, Python, PHP, Java, C#, VBA, VB Script, entre outras), inglês avançado.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Estudantes de graduação a partir do 6º período com conhecimentos em programação e inglês avançado.</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>RPA (Robotic Process Automation), programação, Business Analytics.</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Desenvolver soluções em RPA em conjunto com seu time para clientes nacionais e/ou internacionais, contribuir para uma entrega de soluções de automação, ajudando aos clientes nas suas transformações digitais.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Radix</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Estágio em Desenvolvimento de Negócios</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Remoto</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Cursando Engenharia de Processos, Mecânica, Automação ou áreas correlatas com formação prevista para a partir de 2025/2; Inglês Avançado/Fluente; Excel Intermediário/Avançado; Capacidade de gerenciamento de tempo e resolução de problemas; Vontade de aprender e se desenvolver. Diferencial: Conhecimentos da indústria de Óleo &amp; Gás; Conhecimentos básicos de automação.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Estudantes de Engenharia de Processos, Mecânica, Automação ou áreas correlatas.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Desenvolvimento de Negócios.</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Apoiar no mapeamento e prospecção de oportunidades; Realizar pesquisas de mercado e ações de pré-venda; Elaborar e apresentar propostas técnicas-comerciais nas áreas de atuação da empresa; Acompanhar a equipe técnica nas estimativas de recursos para projetos; Representar a empresa em visitas técnicas e reuniões para a discussão de escopo de projetos; Apoiar na construção, formalização e conclusão de propostas comerciais e orçamentárias; Elaborar materiais de divulgação de soluções desenvolvidas pela Radix.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>Liv Up</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Estágio em Growth - Business Intelligence</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Remoto (Anywhere Office), qualquer lugar do Brasil</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Formatura a partir de Dez/25, Capacidade de resolução de problemas de forma analítica e criativa, Pró atividade, ser mão-na-massa e ter alta capacidade de implementação, Boa comunicação, Excel &amp; PowerPoint avançado, Inglês avançado, SQL e Python são diferenciais</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>A combinar</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Remoto - Anywhere Office (qualquer lugar do Brasil)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Formatura a partir de Dez/25, capacidade de resolução de problemas de forma analítica e criativa, pró-atividade, boa comunicação, Excel &amp; PowerPoint avançado, Inglês avançado, SQL e Python como diferenciais</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>A combinar</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
         <is>
           <t>Estudantes com formatura a partir de Dez/25</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Business Intelligence, Growth, Estratégia de Crescimento, Marketing</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Elaborar modelos de projeção de receita e custos, Elaborar modelos de projeção por canais de marketing, Auxiliar na resolução de problemas relacionados a múltiplas áreas, Acompanhar a performance de testes de Growth, Capacidade de identificar processos recorrentes e automatizá-los, Explicar principais resultados, e alinhar planos de ação com os times responsáveis, Elaborar apresentações para explicar modelagem e resultados dos projetos a serem desenvolvidos.</t>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Growth, Business Intelligence</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Elaboração de modelos de projeção de receita e custos, estratégia e implementação de campanhas de marketing, análise de performance de testes de Growth, automatização de processos recorrentes, alinhamento de planos de ação com times responsáveis.</t>
         </is>
       </c>
     </row>

</xml_diff>